<commit_message>
brandon updated project mgmt file, and added  dump file
</commit_message>
<xml_diff>
--- a/_proj mgmt/vipers_proj_1_mgmt.xlsx
+++ b/_proj mgmt/vipers_proj_1_mgmt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\Documents\_git\repos\Data_Sci_Proj_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\Documents\_git\repos\viper_proj_1\_proj mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3DD219-8901-4081-AB48-6757FCC592B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B51D05-B3FF-4E76-AA15-309348DD064F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="375" windowWidth="20160" windowHeight="15825" xr2:uid="{597B3DE0-42F2-41BC-B04C-FAF8AF40CF76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{597B3DE0-42F2-41BC-B04C-FAF8AF40CF76}"/>
   </bookViews>
   <sheets>
     <sheet name="PROJ MGMT TRACKING" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,71 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>brandon steinke</author>
+  </authors>
+  <commentList>
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{16BCB6B9-5060-4CB3-BA8B-1C06B57601AC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>brandon steinke:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+DATA CLEANING NOTES 
+FROM RON:
+*ucdavis_drg_clean - only has DRG total description
+*ucsd AND  ucsf_drg_clean -- WIll need to string separate DRG code from total description
+*Mass. hospitals have MS### as the drg code. Needs stripping in Python
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="0" shapeId="0" xr:uid="{CB26998D-44C8-4EEB-8652-86BAB371E4A3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>brandon steinke:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="244">
   <si>
     <t xml:space="preserve">Tyler </t>
   </si>
@@ -614,13 +677,166 @@
   </si>
   <si>
     <t>https://github.com/BrandinO771/viper_proj_1.git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">provide data files </t>
+  </si>
+  <si>
+    <t>cleaned / formatted data files</t>
+  </si>
+  <si>
+    <t>merge / grouped data files</t>
+  </si>
+  <si>
+    <t>data dump/CA UC Health Data.zip </t>
+  </si>
+  <si>
+    <t>Dumper</t>
+  </si>
+  <si>
+    <t>Cleaner</t>
+  </si>
+  <si>
+    <t>Merger</t>
+  </si>
+  <si>
+    <t>API puller</t>
+  </si>
+  <si>
+    <t>locator</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>ata dump/MA Partners Healthcare Data.zip</t>
+  </si>
+  <si>
+    <t>data dump/MI McLaren Healthcare Data.zip</t>
+  </si>
+  <si>
+    <t>data dump/nyp_hudson_valley_drg.xlsx </t>
+  </si>
+  <si>
+    <t>CDH_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>MGH_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>MVH_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>NCH_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>NSMC_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>NWH_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>Payment_and_value_of_care_-_Hospital_CLEAN.xlsx</t>
+  </si>
+  <si>
+    <t>mclaren_health_drg_clean.csv</t>
+  </si>
+  <si>
+    <t>nyp_hudson_valley_drg_clean.xlsx</t>
+  </si>
+  <si>
+    <t>ucdavis_drg_clean.csv</t>
+  </si>
+  <si>
+    <t>ucsd_drg_clean.csv</t>
+  </si>
+  <si>
+    <t>ucsf_drg_clean.csv</t>
+  </si>
+  <si>
+    <t>https://health.ucdavis.edu/newsroom/public-reporting/chargemaster.html</t>
+  </si>
+  <si>
+    <t>https://www.verywellhealth.com/how-does-a-drg-determine-how-much-a-hospital-gets-paid-1738874</t>
+  </si>
+  <si>
+    <t>How a DRG Determines How Much a Hospital Gets Paid</t>
+  </si>
+  <si>
+    <t>Top 10 Inpatient Diagnoses by DRG Codes</t>
+  </si>
+  <si>
+    <t>https://blog.definitivehc.com/top-10-inpatient-diagnoses-by-drg-codes</t>
+  </si>
+  <si>
+    <t>https://www.hiacode.com/education/most-common-drgs-with-recommendations-2018-part-1/</t>
+  </si>
+  <si>
+    <t>WEB BLOG/ARTICLE</t>
+  </si>
+  <si>
+    <t>XLSX</t>
+  </si>
+  <si>
+    <t>PYMT AMTS, NO DRG, NAT PROVDRS, PYMT AMT CATEGRZD, PROCEDURE RESULT CATEGRZD</t>
+  </si>
+  <si>
+    <t>DATA CHARTED</t>
+  </si>
+  <si>
+    <t>MEDIAN DRG CHARGES  /DRG CODES / SINGLE MED FACILITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIAN DRG CHARGES  /DRG CODES /NEWTON-WELLESLEY HOSPITAL/HOSP CHGS/PHARMCY CHGS </t>
+  </si>
+  <si>
+    <t>MEDIAN DRG CHARGES  / !!NO DRG CODES /DRG DESCRIP</t>
+  </si>
+  <si>
+    <t>PROJ MGMT UPDATOR</t>
+  </si>
+  <si>
+    <t>MEDIAN DRG CHARGES  /DRG CODES / 11  MED FACILITIES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEE DESCRIPTS BELOW </t>
+  </si>
+  <si>
+    <t>Hospital_Compare_Scores___Ratings</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>hospital scores/ratings/ Zip codes National/ Faclty Name</t>
+  </si>
+  <si>
+    <t>2018/2019</t>
+  </si>
+  <si>
+    <t>1994-2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">871 (Septicemia)        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">291 (Heart Failure)    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">392 GI / Digestive disorders   </t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470 (major joint replace)   [ specify knee  or hip ] </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,8 +967,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,8 +1073,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -955,12 +1209,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFEAECEF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1123,15 +1399,95 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6600"/>
+      <color rgb="FFFF9966"/>
+      <color rgb="FFFF3300"/>
       <color rgb="FFFE750E"/>
       <color rgb="FFD4AE0A"/>
       <color rgb="FFF52C0B"/>
@@ -1493,14 +1849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB40B94-DE18-47E2-9F6F-A7789D179A51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DB40B94-DE18-47E2-9F6F-A7789D179A51}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,7 +1871,7 @@
     <col min="8" max="8" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="19"/>
       <c r="C1" s="8"/>
@@ -1527,7 +1883,7 @@
       <c r="G1" s="25"/>
       <c r="H1" s="26"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="17"/>
       <c r="C2" s="10" t="s">
@@ -1549,7 +1905,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="18" t="s">
         <v>61</v>
@@ -1573,7 +1929,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="18" t="s">
         <v>62</v>
@@ -1597,7 +1953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="18" t="s">
         <v>63</v>
@@ -1621,7 +1977,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="18" t="s">
         <v>63</v>
@@ -1645,7 +2001,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="18" t="s">
         <v>64</v>
@@ -1654,13 +2010,13 @@
         <v>101</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>180</v>
@@ -1669,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="18" t="s">
         <v>65</v>
@@ -1693,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="18" t="s">
         <v>66</v>
@@ -1717,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="35" t="s">
         <v>67</v>
@@ -1741,7 +2097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="18"/>
       <c r="C11" s="31"/>
@@ -1751,7 +2107,7 @@
       <c r="G11" s="32"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="18" t="s">
         <v>6</v>
@@ -1761,20 +2117,20 @@
       </c>
       <c r="D12" s="3">
         <f>SUM(D3:D10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ref="E12:F12" si="0">SUM(E3:E10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38"/>
       <c r="B13" s="19"/>
       <c r="C13" s="8"/>
@@ -1784,7 +2140,7 @@
       <c r="G13" s="27"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="20"/>
       <c r="C14" s="39" t="s">
@@ -1804,7 +2160,7 @@
       </c>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
       <c r="B15" s="20" t="s">
         <v>68</v>
@@ -1825,7 +2181,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
       <c r="B16" s="20" t="s">
         <v>69</v>
@@ -1834,7 +2190,7 @@
         <v>106</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1846,7 +2202,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="20"/>
       <c r="C17" s="7" t="s">
@@ -1865,7 +2221,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="38"/>
       <c r="B18" s="20" t="s">
         <v>70</v>
@@ -1874,7 +2230,7 @@
         <v>182</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -1886,7 +2242,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="38"/>
       <c r="B19" s="20" t="s">
         <v>71</v>
@@ -1907,7 +2263,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="38"/>
       <c r="B20" s="20" t="s">
         <v>72</v>
@@ -1928,7 +2284,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="38"/>
       <c r="B21" s="34"/>
       <c r="C21" s="31"/>
@@ -1937,7 +2293,7 @@
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="38"/>
       <c r="B22" s="20" t="s">
         <v>6</v>
@@ -1947,7 +2303,7 @@
       </c>
       <c r="D22" s="3">
         <f>SUM(D15:D21)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" ref="E22:F22" si="1">SUM(E15:E21)</f>
@@ -1958,7 +2314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38"/>
       <c r="B23" s="19"/>
       <c r="C23" s="8" t="s">
@@ -1972,7 +2328,7 @@
       </c>
       <c r="H23" s="25"/>
     </row>
-    <row r="24" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="38"/>
       <c r="B24" s="21"/>
       <c r="C24" s="40" t="s">
@@ -1992,7 +2348,7 @@
       </c>
       <c r="H24" s="25"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="38"/>
       <c r="B25" s="21" t="s">
         <v>73</v>
@@ -2013,7 +2369,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="38"/>
       <c r="B26" s="21" t="s">
         <v>74</v>
@@ -2034,7 +2390,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="38"/>
       <c r="B27" s="21"/>
       <c r="C27" s="7" t="s">
@@ -2053,7 +2409,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="38"/>
       <c r="B28" s="21"/>
       <c r="C28" s="7" t="s">
@@ -2072,7 +2428,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="38"/>
       <c r="B29" s="21"/>
       <c r="D29" s="30" t="s">
@@ -2088,7 +2444,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="38"/>
       <c r="B30" s="21" t="s">
         <v>75</v>
@@ -2109,7 +2465,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="38"/>
       <c r="B31" s="21" t="s">
         <v>76</v>
@@ -2130,7 +2486,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="38"/>
       <c r="B32" s="21" t="s">
         <v>78</v>
@@ -2504,6 +2860,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2515,7 +2872,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2555,34 +2912,57 @@
       <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="2">
+        <v>871</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" s="2">
+        <v>470</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
       <c r="B6" s="18">
         <v>3</v>
       </c>
+      <c r="C6" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6">
+        <v>291</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="18">
         <v>4</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="2">
+        <v>392</v>
+      </c>
     </row>
     <row r="8" spans="1:4" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="18">
         <v>5</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
@@ -2948,459 +3328,1945 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" customWidth="1"/>
-    <col min="9" max="9" width="98.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.42578125" customWidth="1"/>
+    <col min="2" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="53.42578125" customWidth="1"/>
+    <col min="10" max="10" width="41.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="25.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="48"/>
-      <c r="B1" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="48"/>
       <c r="G1" s="48"/>
       <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-    </row>
-    <row r="2" spans="1:10" s="14" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="53" t="s">
+      <c r="I1" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+    </row>
+    <row r="2" spans="1:17" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+    </row>
+    <row r="3" spans="1:17" s="14" customFormat="1" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="52"/>
+      <c r="B3" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>227</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>200</v>
+      </c>
+      <c r="G3" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="H3" s="66" t="s">
+        <v>231</v>
+      </c>
+      <c r="I3" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="J3" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="K3" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="L3" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="M3" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="N3" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="O3" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="P3" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="Q3" s="56" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="J4" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="M4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N4" t="s">
         <v>139</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="P4" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="J5" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F4" t="s">
+      <c r="M5" t="s">
         <v>136</v>
       </c>
-      <c r="G4" t="s">
+      <c r="N5" t="s">
         <v>136</v>
       </c>
-      <c r="H4" t="s">
+      <c r="O5" t="s">
         <v>136</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="J4" t="s">
+      <c r="Q5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="C5" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="J6" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="M6" t="s">
+        <v>127</v>
+      </c>
+      <c r="N6" t="s">
         <v>139</v>
       </c>
-      <c r="H5" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="9" t="s">
+      <c r="O6" t="s">
+        <v>127</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="60" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="J7" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H6" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="9" t="s">
+      <c r="M7" t="s">
+        <v>136</v>
+      </c>
+      <c r="N7" t="s">
+        <v>136</v>
+      </c>
+      <c r="O7" t="s">
+        <v>136</v>
+      </c>
+      <c r="P7" s="9" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="60" t="s">
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="J8" s="51" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="9" t="s">
+      <c r="K8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M8" t="s">
+        <v>136</v>
+      </c>
+      <c r="N8" t="s">
+        <v>136</v>
+      </c>
+      <c r="O8" t="s">
+        <v>136</v>
+      </c>
+      <c r="P8" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="J9" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="M9" t="s">
+        <v>136</v>
+      </c>
+      <c r="N9" t="s">
+        <v>136</v>
+      </c>
+      <c r="O9" t="s">
+        <v>136</v>
+      </c>
+      <c r="P9" t="s">
         <v>148</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="Q9" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="J10" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F9" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" t="s">
-        <v>127</v>
-      </c>
-      <c r="H9" t="s">
-        <v>127</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="M10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N10" t="s">
+        <v>136</v>
+      </c>
+      <c r="O10" t="s">
+        <v>136</v>
+      </c>
+      <c r="P10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="J11" s="59" t="s">
         <v>154</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="K11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" t="s">
-        <v>127</v>
-      </c>
-      <c r="H10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="9" t="s">
+      <c r="M11" t="s">
+        <v>136</v>
+      </c>
+      <c r="N11" t="s">
+        <v>136</v>
+      </c>
+      <c r="O11" t="s">
+        <v>136</v>
+      </c>
+      <c r="P11" s="9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I12" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="J12" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F11" t="s">
-        <v>127</v>
-      </c>
-      <c r="G11" t="s">
-        <v>127</v>
-      </c>
-      <c r="H11" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="M12" t="s">
+        <v>136</v>
+      </c>
+      <c r="N12" t="s">
+        <v>136</v>
+      </c>
+      <c r="O12" t="s">
+        <v>136</v>
+      </c>
+      <c r="P12" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="J13" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="K13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F12" t="s">
-        <v>127</v>
-      </c>
-      <c r="G12" t="s">
-        <v>127</v>
-      </c>
-      <c r="H12" t="s">
-        <v>127</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="M13" t="s">
+        <v>136</v>
+      </c>
+      <c r="N13" t="s">
+        <v>136</v>
+      </c>
+      <c r="O13" t="s">
+        <v>136</v>
+      </c>
+      <c r="P13" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="J14" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" t="s">
-        <v>127</v>
-      </c>
-      <c r="H13" t="s">
-        <v>127</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="M14" t="s">
+        <v>136</v>
+      </c>
+      <c r="N14" t="s">
+        <v>136</v>
+      </c>
+      <c r="O14" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="J15" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="M15" t="s">
+        <v>136</v>
+      </c>
+      <c r="N15" t="s">
+        <v>136</v>
+      </c>
+      <c r="O15" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q15" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" t="s">
-        <v>127</v>
-      </c>
-      <c r="G15" t="s">
-        <v>127</v>
-      </c>
-      <c r="H15" t="s">
-        <v>127</v>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="J16" t="s">
+        <v>196</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="J17" t="s">
+        <v>203</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="J18" t="s">
+        <v>204</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="J19" t="s">
+        <v>205</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J20" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J21" s="68" t="s">
+        <v>207</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I22" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J22" s="69" t="s">
+        <v>208</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J23" s="69" t="s">
+        <v>209</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I24" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J24" s="69" t="s">
+        <v>210</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="J25" s="69" t="s">
+        <v>211</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="73" t="s">
+        <v>226</v>
+      </c>
+      <c r="J26" s="69" t="s">
+        <v>212</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="J27" s="69" t="s">
+        <v>213</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I28" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J28" s="69" t="s">
+        <v>214</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I29" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="J29" s="69" t="s">
+        <v>215</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J30" s="69" t="s">
+        <v>216</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P30" s="70" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I31" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="J31" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P31" s="70" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I32" s="72" t="s">
+        <v>220</v>
+      </c>
+      <c r="J32" s="72" t="s">
+        <v>220</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L32" s="71" t="s">
+        <v>224</v>
+      </c>
+      <c r="M32" t="s">
+        <v>136</v>
+      </c>
+      <c r="N32" t="s">
+        <v>136</v>
+      </c>
+      <c r="O32" t="s">
+        <v>136</v>
+      </c>
+      <c r="P32" s="70" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="J33" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L33" s="71" t="s">
+        <v>224</v>
+      </c>
+      <c r="M33" t="s">
+        <v>136</v>
+      </c>
+      <c r="N33" t="s">
+        <v>136</v>
+      </c>
+      <c r="O33" t="s">
+        <v>136</v>
+      </c>
+      <c r="P33" s="70" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I34" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="J34" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L34" s="71" t="s">
+        <v>224</v>
+      </c>
+      <c r="M34" t="s">
+        <v>136</v>
+      </c>
+      <c r="N34" t="s">
+        <v>136</v>
+      </c>
+      <c r="O34" t="s">
+        <v>136</v>
+      </c>
+      <c r="P34" s="70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I35" s="57" t="s">
+        <v>236</v>
+      </c>
+      <c r="J35" t="s">
+        <v>234</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>32</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>32</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>32</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>32</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>32</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>32</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="B4:H41">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{F05A3756-57CE-474C-815A-7E95FB5ECAD0}"/>
-    <hyperlink ref="I4" r:id="rId2" xr:uid="{7F2E12EA-731E-4F3D-B7D9-2534FAAE76A3}"/>
-    <hyperlink ref="I5" r:id="rId3" xr:uid="{CB5216E9-EA6D-4D0C-98EE-FF1B192EFE3D}"/>
-    <hyperlink ref="I6" r:id="rId4" xr:uid="{C3A90F8F-CCFE-4B41-A698-A28A88D92DBD}"/>
-    <hyperlink ref="I7" r:id="rId5" xr:uid="{8ECD68E4-8370-47FE-8CAD-D462504DB95B}"/>
-    <hyperlink ref="J8" r:id="rId6" xr:uid="{8B1687AD-BBBD-44B8-B9F3-06FE3AC6CF53}"/>
-    <hyperlink ref="I10" r:id="rId7" xr:uid="{618DBDAB-197A-4D91-838C-DB3B3EF63978}"/>
-    <hyperlink ref="I11" r:id="rId8" xr:uid="{DC0084DB-D45B-4A5D-9ACF-D2D92B2476E4}"/>
-    <hyperlink ref="I12" r:id="rId9" xr:uid="{9C5F7808-808A-43B9-AC76-2E355A9E4F33}"/>
+    <hyperlink ref="P4" r:id="rId1" xr:uid="{F05A3756-57CE-474C-815A-7E95FB5ECAD0}"/>
+    <hyperlink ref="P5" r:id="rId2" xr:uid="{7F2E12EA-731E-4F3D-B7D9-2534FAAE76A3}"/>
+    <hyperlink ref="P6" r:id="rId3" xr:uid="{CB5216E9-EA6D-4D0C-98EE-FF1B192EFE3D}"/>
+    <hyperlink ref="P7" r:id="rId4" xr:uid="{C3A90F8F-CCFE-4B41-A698-A28A88D92DBD}"/>
+    <hyperlink ref="P8" r:id="rId5" xr:uid="{8ECD68E4-8370-47FE-8CAD-D462504DB95B}"/>
+    <hyperlink ref="Q9" r:id="rId6" xr:uid="{8B1687AD-BBBD-44B8-B9F3-06FE3AC6CF53}"/>
+    <hyperlink ref="P11" r:id="rId7" xr:uid="{618DBDAB-197A-4D91-838C-DB3B3EF63978}"/>
+    <hyperlink ref="P12" r:id="rId8" xr:uid="{DC0084DB-D45B-4A5D-9ACF-D2D92B2476E4}"/>
+    <hyperlink ref="P13" r:id="rId9" xr:uid="{9C5F7808-808A-43B9-AC76-2E355A9E4F33}"/>
+    <hyperlink ref="P31" r:id="rId10" xr:uid="{944A0C99-351C-4179-9EED-B8F6ACD5DE96}"/>
+    <hyperlink ref="P30" r:id="rId11" xr:uid="{15F29AA1-6354-4962-9ABA-AD75BB54B3F5}"/>
+    <hyperlink ref="P32" r:id="rId12" xr:uid="{0C7209B5-A305-4D2E-A103-7024E46377DE}"/>
+    <hyperlink ref="P33" r:id="rId13" xr:uid="{D178F96C-97FF-4DEB-B71B-FB06A6F0EC12}"/>
+    <hyperlink ref="P34" r:id="rId14" xr:uid="{4AA03050-EAFB-44B2-8281-D3B8A652DFC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -4475,7 +6341,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4582,6 +6448,30 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
brandon updata proj mgmt, upload dump Inpatient_PYMT_IPPS_DRG_FY2017, upload clean Inpatient_PYMT_IPPS_DRG_FY2017_clean, updated Jupyter Data_Analysis.ipyn
</commit_message>
<xml_diff>
--- a/_proj mgmt/vipers_proj_1_mgmt.xlsx
+++ b/_proj mgmt/vipers_proj_1_mgmt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\Documents\_git\repos\viper_proj_1\_proj mgmt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B51D05-B3FF-4E76-AA15-309348DD064F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD238B8-3EBF-4C93-81D5-4F3DE5DDDBCD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{597B3DE0-42F2-41BC-B04C-FAF8AF40CF76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="1000" xr2:uid="{597B3DE0-42F2-41BC-B04C-FAF8AF40CF76}"/>
   </bookViews>
   <sheets>
     <sheet name="PROJ MGMT TRACKING" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="data reference links " sheetId="3" r:id="rId3"/>
     <sheet name="Project Guidelines " sheetId="2" r:id="rId4"/>
     <sheet name="contributions" sheetId="5" r:id="rId5"/>
+    <sheet name="TERMS" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="282">
   <si>
     <t xml:space="preserve">Tyler </t>
   </si>
@@ -830,13 +831,619 @@
   </si>
   <si>
     <t xml:space="preserve">470 (major joint replace)   [ specify knee  or hip ] </t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>major complication or comorbidity</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>https://www.cms.gov/icd10manual/fullcode_cms/p0031.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIST OF ALL DRG CODES </t>
+  </si>
+  <si>
+    <t>major joint replace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heart Failure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Septicemia      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GI / Digestive disorders   </t>
+  </si>
+  <si>
+    <t>871 - SEPTICEMIA OR SEVERE SEPSIS W/O MV 96+ HOURS W MCC</t>
+  </si>
+  <si>
+    <t>470 - MAJOR JOINT REPLACEMENT OR REATTACHMENT OF LOWER EXTREMITY W/O MCC</t>
+  </si>
+  <si>
+    <t>291 - HEART FAILURE &amp; SHOCK W MCC</t>
+  </si>
+  <si>
+    <t>392 - ESOPHAGITIS, GASTROENT &amp; MISC DIGEST DISORDERS W/O MCC</t>
+  </si>
+  <si>
+    <t>DRG CODE</t>
+  </si>
+  <si>
+    <t>SHORT DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG DEF </t>
+  </si>
+  <si>
+    <t>the simultaneous presence of two chronic diseases or conditions in a patient.</t>
+  </si>
+  <si>
+    <t>280 - ACUTE MYOCARDIAL INFARCTION, DISCHARGED ALIVE W MCC</t>
+  </si>
+  <si>
+    <t>303 - ATHEROSCLEROSIS W/O MCC</t>
+  </si>
+  <si>
+    <t>418 - LAPAROSCOPIC CHOLECYSTECTOMY W/O C.D.E. W CC</t>
+  </si>
+  <si>
+    <t>638 - DIABETES W CC</t>
+  </si>
+  <si>
+    <t>664 - MINOR BLADDER PROCEDURES W/O CC/MCC</t>
+  </si>
+  <si>
+    <t>complication or comorbidity </t>
+  </si>
+  <si>
+    <r>
+      <t>Gastroenterology Disease It includes common and important conditions such as colon polyps and cancer, hepatitis, gastroesophageal reflux (heartburn), peptic ulcer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>disease</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, colitis, gallbladder and biliary tract </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>disease</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Eosinophilic </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Esophagitis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (EoE) Eosinophilic (ee-uh-sin-uh-fil-ik) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>esophagitis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (EoE) is a recognized chronic allergic/immune condition. A person with EoE will have inflammation of the esophagus. ... </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Acute myocardial infarction is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> the medical name for a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>heart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> attack. A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>heart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> attack </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a life-threatening condition that occurs when blood flow to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>heart</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> muscle </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>abruptly cut off, causing tissue damage. This </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> usually the result of a blockage in one or more of the coronary arteries.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Atherosclerosis is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> a disease in which plaque builds up inside your arteries. Arteries </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>are</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> blood vessels that carry oxygen-rich blood to your heart and other parts of your body. Plaque </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> made up of fat, cholesterol, calcium, and other substances </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>laparoscopic cholecystectomy is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>surgery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> during which the doctor removes your</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>gallbladder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Diabetes is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> a disease that occurs when your blood glucose, also called blood sugar, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> too high. ... Insulin, a hormone made by the pancreas, helps glucose from food get into your cells to be used for energy.</t>
+    </r>
+  </si>
+  <si>
+    <t>SELECTED DRG CODES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONGER DEFINITIONS AND OTHER CODES </t>
+  </si>
+  <si>
+    <t>ABBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (MCC) when used as a secondary diagnosis</t>
+  </si>
+  <si>
+    <t>Part 2 lists codes which are assigned as a Major CC only for patients discharged alive.</t>
+  </si>
+  <si>
+    <t>PART 2</t>
+  </si>
+  <si>
+    <t>WITHIN THE DRG CODE DEFINITION YOU WILL SEE     'WITH CC  OR MCC '</t>
+  </si>
+  <si>
+    <r>
+      <t>Appendix C </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> a list </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> all </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>codes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>are</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> defined as either a complication or comorbidity (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) or a major complication or comorbidity (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MCC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF222222"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) when used as a secondary diagnosis. …</t>
+    </r>
+  </si>
+  <si>
+    <t>https://dev.socrata.com/foundry/data.medicare.gov/vv6z-qryr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -993,8 +1600,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1082,6 +1748,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF6F8FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1236,7 +1908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1419,19 +2091,50 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -1449,28 +2152,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3300"/>
+          <bgColor rgb="FFFF6600"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1485,6 +2167,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9F399F"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFFF9966"/>
       <color rgb="FFFF3300"/>
@@ -1856,7 +2539,7 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,7 +3555,7 @@
   <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3331,10 +4014,10 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3487,6 +4170,9 @@
       <c r="P4" s="9" t="s">
         <v>57</v>
       </c>
+      <c r="Q4" s="9" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -5076,6 +5762,9 @@
       <c r="L35" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="P35" s="9" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -5096,11 +5785,14 @@
       <c r="F36" s="1">
         <v>0</v>
       </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0</v>
+      <c r="G36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="72" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -5239,13 +5931,13 @@
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"T"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"B"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5264,9 +5956,11 @@
     <hyperlink ref="P32" r:id="rId12" xr:uid="{0C7209B5-A305-4D2E-A103-7024E46377DE}"/>
     <hyperlink ref="P33" r:id="rId13" xr:uid="{D178F96C-97FF-4DEB-B71B-FB06A6F0EC12}"/>
     <hyperlink ref="P34" r:id="rId14" xr:uid="{4AA03050-EAFB-44B2-8281-D3B8A652DFC5}"/>
+    <hyperlink ref="P35" r:id="rId15" xr:uid="{D4DD0576-1F93-49E5-9F7E-62EFA1C21CD4}"/>
+    <hyperlink ref="Q4" r:id="rId16" xr:uid="{8D96480A-790C-4C8C-BDF2-9C059D5759F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -6338,6 +7032,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1B8710-602E-49E5-B1A4-B3BB84C29D63}">
+  <sheetPr>
+    <tabColor rgb="FF9F399F"/>
+  </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6480,4 +7177,251 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3956EFEA-0FE2-435B-94D3-64ABF093CBDF}">
+  <sheetPr>
+    <tabColor theme="3" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="B1:D27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" style="74" customWidth="1"/>
+    <col min="3" max="3" width="67" customWidth="1"/>
+    <col min="4" max="4" width="80.5703125" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" s="83" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="78" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" s="82"/>
+    </row>
+    <row r="3" spans="2:4" s="83" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B3" s="91" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" s="83" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="85" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="88" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" s="83" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="85" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="85" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" s="83" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="86" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" s="83" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="89" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" s="86"/>
+    </row>
+    <row r="8" spans="2:4" s="83" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+    </row>
+    <row r="9" spans="2:4" s="90" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="78" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="79"/>
+    </row>
+    <row r="11" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="80" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="75">
+        <v>871</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="D12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="75">
+        <v>470</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="75">
+        <v>291</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="75">
+        <v>392</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="74">
+        <v>638</v>
+      </c>
+      <c r="C16" s="74" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="78" t="s">
+        <v>274</v>
+      </c>
+      <c r="C18" s="79"/>
+    </row>
+    <row r="19" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="80" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="81" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="74">
+        <v>392</v>
+      </c>
+      <c r="C20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" s="76" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="74">
+        <v>392</v>
+      </c>
+      <c r="C21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" s="76" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="74">
+        <v>280</v>
+      </c>
+      <c r="C22" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="D22" s="77" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="74">
+        <v>303</v>
+      </c>
+      <c r="C23" s="74" t="s">
+        <v>262</v>
+      </c>
+      <c r="D23" s="77" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="74">
+        <v>418</v>
+      </c>
+      <c r="C24" s="74" t="s">
+        <v>263</v>
+      </c>
+      <c r="D24" s="76" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="74">
+        <v>638</v>
+      </c>
+      <c r="C25" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="D25" s="77" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="74">
+        <v>664</v>
+      </c>
+      <c r="C26" s="74" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="74"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>